<commit_message>
added function to delete pickle files
</commit_message>
<xml_diff>
--- a/graphs/2014/datafigures.xlsx
+++ b/graphs/2014/datafigures.xlsx
@@ -903,13 +903,20 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:rPr lang="en-US"/>
+              <a:rPr lang="en-US" sz="2400"/>
               <a:t>COMPONENT SIZES</a:t>
             </a:r>
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.2131387638064097"/>
+          <c:y val="8.1355810598548149E-3"/>
+        </c:manualLayout>
+      </c:layout>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -974,7 +981,7 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
                       <a:schemeClr val="tx1">
                         <a:lumMod val="50000"/>
@@ -1113,11 +1120,11 @@
         </c:dLbls>
         <c:gapWidth val="444"/>
         <c:overlap val="-90"/>
-        <c:axId val="317414672"/>
-        <c:axId val="317415848"/>
+        <c:axId val="417057328"/>
+        <c:axId val="417062032"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="317414672"/>
+        <c:axId val="417057328"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1157,13 +1164,20 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="en-US" sz="1200"/>
+                  <a:rPr lang="en-US" sz="2000" b="1" cap="none" baseline="0"/>
                   <a:t>Component size</a:t>
                 </a:r>
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
+          <c:layout>
+            <c:manualLayout>
+              <c:xMode val="edge"/>
+              <c:yMode val="edge"/>
+              <c:x val="0.33580209927729832"/>
+              <c:y val="0.83966787611367777"/>
+            </c:manualLayout>
+          </c:layout>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -1215,7 +1229,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="all" spc="120" normalizeH="0" baseline="0">
+              <a:defRPr sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" spc="120" normalizeH="0" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -1230,7 +1244,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="317415848"/>
+        <c:crossAx val="417062032"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1238,7 +1252,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="317415848"/>
+        <c:axId val="417062032"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1264,13 +1278,20 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="en-US" sz="1200"/>
+                  <a:rPr lang="en-US" sz="2000" b="1" cap="none" baseline="0"/>
                   <a:t>Frequency</a:t>
                 </a:r>
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
+          <c:layout>
+            <c:manualLayout>
+              <c:xMode val="edge"/>
+              <c:yMode val="edge"/>
+              <c:x val="2.1710324862104179E-2"/>
+              <c:y val="0.27863756562915581"/>
+            </c:manualLayout>
+          </c:layout>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -1304,7 +1325,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="317414672"/>
+        <c:crossAx val="417057328"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1393,7 +1414,14 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.1022303107515635"/>
+          <c:y val="3.8493083671840098E-3"/>
+        </c:manualLayout>
+      </c:layout>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1430,9 +1458,9 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="5.7725344242498637E-2"/>
-          <c:y val="0.16912037037037039"/>
-          <c:w val="0.8818252515101026"/>
+          <c:x val="0.10421927925518341"/>
+          <c:y val="0.1883669657811641"/>
+          <c:w val="0.82712642074178011"/>
           <c:h val="0.44626062424264107"/>
         </c:manualLayout>
       </c:layout>
@@ -1468,7 +1496,7 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
                       <a:schemeClr val="tx1">
                         <a:lumMod val="50000"/>
@@ -1600,11 +1628,11 @@
         </c:dLbls>
         <c:gapWidth val="444"/>
         <c:overlap val="-90"/>
-        <c:axId val="317415456"/>
-        <c:axId val="317416240"/>
+        <c:axId val="417061248"/>
+        <c:axId val="417059288"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="317415456"/>
+        <c:axId val="417061248"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1650,7 +1678,14 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
+          <c:layout>
+            <c:manualLayout>
+              <c:xMode val="edge"/>
+              <c:yMode val="edge"/>
+              <c:x val="0.22417070500922448"/>
+              <c:y val="0.88701370656873868"/>
+            </c:manualLayout>
+          </c:layout>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -1698,11 +1733,11 @@
           <a:effectLst/>
         </c:spPr>
         <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:bodyPr rot="-3600000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="all" spc="120" normalizeH="0" baseline="0">
+              <a:defRPr sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" spc="120" normalizeH="0" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -1717,7 +1752,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="317416240"/>
+        <c:crossAx val="417059288"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1725,7 +1760,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="317416240"/>
+        <c:axId val="417059288"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1761,8 +1796,8 @@
             <c:manualLayout>
               <c:xMode val="edge"/>
               <c:yMode val="edge"/>
-              <c:x val="1.9825852407119152E-2"/>
-              <c:y val="0.38871925030803134"/>
+              <c:x val="5.7842890869674109E-4"/>
+              <c:y val="0.28478789704706525"/>
             </c:manualLayout>
           </c:layout>
           <c:overlay val="0"/>
@@ -1798,7 +1833,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="317415456"/>
+        <c:crossAx val="417061248"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2204,11 +2239,11 @@
         </c:dLbls>
         <c:gapWidth val="444"/>
         <c:overlap val="-90"/>
-        <c:axId val="320402424"/>
-        <c:axId val="320397720"/>
+        <c:axId val="417060856"/>
+        <c:axId val="417062816"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="320402424"/>
+        <c:axId val="417060856"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2328,7 +2363,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="320397720"/>
+        <c:crossAx val="417062816"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2336,7 +2371,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="320397720"/>
+        <c:axId val="417062816"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2409,7 +2444,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="320402424"/>
+        <c:crossAx val="417060856"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2719,11 +2754,11 @@
         </c:dLbls>
         <c:gapWidth val="444"/>
         <c:overlap val="-90"/>
-        <c:axId val="320398896"/>
-        <c:axId val="320402032"/>
+        <c:axId val="417058112"/>
+        <c:axId val="417063992"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="320398896"/>
+        <c:axId val="417058112"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2843,7 +2878,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="320402032"/>
+        <c:crossAx val="417063992"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2851,7 +2886,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="320402032"/>
+        <c:axId val="417063992"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2925,7 +2960,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="320398896"/>
+        <c:crossAx val="417058112"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3241,8 +3276,8 @@
         </c:dLbls>
         <c:gapWidth val="444"/>
         <c:overlap val="-90"/>
-        <c:axId val="320401640"/>
-        <c:axId val="320402816"/>
+        <c:axId val="418033344"/>
+        <c:axId val="418039224"/>
         <c:extLst>
           <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
             <c15:filteredBarSeries>
@@ -3424,7 +3459,7 @@
         </c:extLst>
       </c:barChart>
       <c:catAx>
-        <c:axId val="320401640"/>
+        <c:axId val="418033344"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3544,7 +3579,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="320402816"/>
+        <c:crossAx val="418039224"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3552,7 +3587,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="320402816"/>
+        <c:axId val="418039224"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3625,7 +3660,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="320401640"/>
+        <c:crossAx val="418033344"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3708,13 +3743,20 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:rPr lang="en-US"/>
+              <a:rPr lang="en-US" sz="2400"/>
               <a:t>Betweenness Centrality</a:t>
             </a:r>
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.2098852260369278"/>
+          <c:y val="2.1365951645654944E-2"/>
+        </c:manualLayout>
+      </c:layout>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -3751,10 +3793,10 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.11256173304083118"/>
-          <c:y val="0.17788822860131437"/>
-          <c:w val="0.85735126516318916"/>
-          <c:h val="0.46558011621873518"/>
+          <c:x val="0.15739985591928793"/>
+          <c:y val="0.18664156923722333"/>
+          <c:w val="0.75059359740284837"/>
+          <c:h val="0.34303365982506701"/>
         </c:manualLayout>
       </c:layout>
       <c:barChart>
@@ -3800,7 +3842,7 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
                       <a:schemeClr val="tx1">
                         <a:lumMod val="50000"/>
@@ -3944,8 +3986,8 @@
         </c:dLbls>
         <c:gapWidth val="444"/>
         <c:overlap val="-90"/>
-        <c:axId val="320398112"/>
-        <c:axId val="320403600"/>
+        <c:axId val="418038048"/>
+        <c:axId val="418034520"/>
         <c:extLst>
           <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
             <c15:filteredBarSeries>
@@ -4104,7 +4146,7 @@
         </c:extLst>
       </c:barChart>
       <c:catAx>
-        <c:axId val="320398112"/>
+        <c:axId val="418038048"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4144,13 +4186,20 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="en-US" sz="1200"/>
+                  <a:rPr lang="en-US" sz="2000" b="1" cap="none" baseline="0"/>
                   <a:t>Betweenness Centrality</a:t>
                 </a:r>
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
+          <c:layout>
+            <c:manualLayout>
+              <c:xMode val="edge"/>
+              <c:yMode val="edge"/>
+              <c:x val="0.30649329907003214"/>
+              <c:y val="0.82664049402695416"/>
+            </c:manualLayout>
+          </c:layout>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -4202,7 +4251,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="all" spc="120" normalizeH="0" baseline="0">
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="all" spc="120" normalizeH="0" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -4217,7 +4266,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="320403600"/>
+        <c:crossAx val="418034520"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4225,7 +4274,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="320403600"/>
+        <c:axId val="418034520"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4238,7 +4287,7 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+                  <a:defRPr sz="2000" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
                     <a:solidFill>
                       <a:schemeClr val="tx1">
                         <a:lumMod val="65000"/>
@@ -4251,8 +4300,8 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="en-US" sz="1200"/>
-                  <a:t>FREQUENCY</a:t>
+                  <a:rPr lang="en-US" sz="2000" b="1" cap="none" baseline="0"/>
+                  <a:t>Frequency</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -4261,8 +4310,8 @@
             <c:manualLayout>
               <c:xMode val="edge"/>
               <c:yMode val="edge"/>
-              <c:x val="5.8859100662764355E-2"/>
-              <c:y val="0.29382486036459166"/>
+              <c:x val="7.1669982876755495E-2"/>
+              <c:y val="0.2763182411030371"/>
             </c:manualLayout>
           </c:layout>
           <c:overlay val="0"/>
@@ -4278,7 +4327,7 @@
             <a:lstStyle/>
             <a:p>
               <a:pPr>
-                <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+                <a:defRPr sz="2000" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
                   <a:solidFill>
                     <a:schemeClr val="tx1">
                       <a:lumMod val="65000"/>
@@ -4298,7 +4347,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="320398112"/>
+        <c:crossAx val="418038048"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4381,7 +4430,7 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:rPr lang="en-US"/>
+              <a:rPr lang="en-US" sz="2400"/>
               <a:t>Closeness Centrality</a:t>
             </a:r>
           </a:p>
@@ -4391,8 +4440,8 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.27889207959091716"/>
-          <c:y val="2.2264253525333007E-2"/>
+          <c:x val="0.19454502332476523"/>
+          <c:y val="6.7603592869562084E-3"/>
         </c:manualLayout>
       </c:layout>
       <c:overlay val="0"/>
@@ -4432,9 +4481,9 @@
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
           <c:x val="0.15920324021061069"/>
-          <c:y val="0.15042883611807079"/>
-          <c:w val="0.54684161142264609"/>
-          <c:h val="0.60639792092309697"/>
+          <c:y val="0.16782055550858954"/>
+          <c:w val="0.6112117919442478"/>
+          <c:h val="0.50562274747520375"/>
         </c:manualLayout>
       </c:layout>
       <c:barChart>
@@ -4469,7 +4518,7 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
                       <a:schemeClr val="tx1">
                         <a:lumMod val="50000"/>
@@ -4613,11 +4662,11 @@
         </c:dLbls>
         <c:gapWidth val="444"/>
         <c:overlap val="-90"/>
-        <c:axId val="320404384"/>
-        <c:axId val="320399680"/>
+        <c:axId val="418038440"/>
+        <c:axId val="418038832"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="320404384"/>
+        <c:axId val="418038440"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4657,7 +4706,7 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="en-US" sz="1200"/>
+                  <a:rPr lang="en-US" sz="2000" b="1" cap="none" baseline="0"/>
                   <a:t>Closeness</a:t>
                 </a:r>
               </a:p>
@@ -4667,8 +4716,8 @@
             <c:manualLayout>
               <c:xMode val="edge"/>
               <c:yMode val="edge"/>
-              <c:x val="0.67341830337354991"/>
-              <c:y val="0.89972147225929089"/>
+              <c:x val="0.71337218376464906"/>
+              <c:y val="0.86273244743562005"/>
             </c:manualLayout>
           </c:layout>
           <c:overlay val="0"/>
@@ -4718,11 +4767,11 @@
           <a:effectLst/>
         </c:spPr>
         <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:bodyPr rot="-3000000" spcFirstLastPara="1" vertOverflow="ellipsis" wrap="square" anchor="ctr" anchorCtr="1"/>
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="all" spc="120" normalizeH="0" baseline="0">
+              <a:defRPr sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" spc="120" normalizeH="0" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -4737,7 +4786,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="320399680"/>
+        <c:crossAx val="418038832"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4745,7 +4794,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="320399680"/>
+        <c:axId val="418038832"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4771,8 +4820,8 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="en-US" sz="1200"/>
-                  <a:t>frequency</a:t>
+                  <a:rPr lang="en-US" sz="2000" b="1" cap="none" baseline="0"/>
+                  <a:t>Frequency</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -4781,8 +4830,8 @@
             <c:manualLayout>
               <c:xMode val="edge"/>
               <c:yMode val="edge"/>
-              <c:x val="0.10623938000676747"/>
-              <c:y val="0.34431265320571969"/>
+              <c:x val="8.6262394039710213E-2"/>
+              <c:y val="0.31718082244374585"/>
             </c:manualLayout>
           </c:layout>
           <c:overlay val="0"/>
@@ -4818,7 +4867,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="320404384"/>
+        <c:crossAx val="418038440"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -8841,15 +8890,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>18</xdr:col>
-      <xdr:colOff>155171</xdr:colOff>
+      <xdr:colOff>173315</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>38991</xdr:rowOff>
+      <xdr:rowOff>48062</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>26</xdr:col>
-      <xdr:colOff>571500</xdr:colOff>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>562428</xdr:colOff>
       <xdr:row>21</xdr:row>
-      <xdr:rowOff>72571</xdr:rowOff>
+      <xdr:rowOff>81642</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -8961,15 +9010,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>19</xdr:col>
-      <xdr:colOff>120730</xdr:colOff>
+      <xdr:colOff>120729</xdr:colOff>
       <xdr:row>21</xdr:row>
-      <xdr:rowOff>128650</xdr:rowOff>
+      <xdr:rowOff>128649</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>28</xdr:col>
-      <xdr:colOff>59377</xdr:colOff>
-      <xdr:row>41</xdr:row>
-      <xdr:rowOff>66501</xdr:rowOff>
+      <xdr:colOff>598713</xdr:colOff>
+      <xdr:row>45</xdr:row>
+      <xdr:rowOff>127000</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -8991,15 +9040,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>15</xdr:col>
-      <xdr:colOff>524490</xdr:colOff>
-      <xdr:row>68</xdr:row>
-      <xdr:rowOff>127659</xdr:rowOff>
+      <xdr:colOff>587990</xdr:colOff>
+      <xdr:row>69</xdr:row>
+      <xdr:rowOff>659</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>25</xdr:col>
-      <xdr:colOff>168234</xdr:colOff>
-      <xdr:row>86</xdr:row>
-      <xdr:rowOff>138546</xdr:rowOff>
+      <xdr:colOff>231734</xdr:colOff>
+      <xdr:row>87</xdr:row>
+      <xdr:rowOff>11545</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -9346,8 +9395,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:S252"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F46" zoomScale="84" zoomScaleNormal="84" workbookViewId="0">
-      <selection activeCell="K29" sqref="K29"/>
+    <sheetView tabSelected="1" topLeftCell="N66" zoomScale="84" zoomScaleNormal="84" workbookViewId="0">
+      <selection activeCell="AA82" sqref="AA82"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -11344,7 +11393,7 @@
     <col min="17" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:17" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B3" s="1" t="s">
         <v>23</v>
       </c>
@@ -11358,7 +11407,7 @@
         <v>1.7999999999999999E-2</v>
       </c>
     </row>
-    <row r="4" spans="2:17" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B4" s="1" t="s">
         <v>24</v>
       </c>
@@ -11372,7 +11421,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="2:17" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B5" s="1" t="s">
         <v>17</v>
       </c>
@@ -11386,7 +11435,7 @@
         <v>1.04</v>
       </c>
     </row>
-    <row r="6" spans="2:17" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B6" s="1" t="s">
         <v>21</v>
       </c>
@@ -11400,7 +11449,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="7" spans="2:17" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B7" s="1" t="s">
         <v>56</v>
       </c>
@@ -11414,7 +11463,7 @@
         <v>4.26</v>
       </c>
     </row>
-    <row r="8" spans="2:17" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:17" x14ac:dyDescent="0.35">
       <c r="E8" s="1" t="s">
         <v>22</v>
       </c>
@@ -11424,16 +11473,16 @@
       <c r="M8" s="4"/>
       <c r="N8" s="4"/>
     </row>
-    <row r="9" spans="2:17" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:17" x14ac:dyDescent="0.35">
       <c r="M9" s="3"/>
       <c r="N9" s="3"/>
     </row>
-    <row r="15" spans="2:17" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:17" x14ac:dyDescent="0.35">
       <c r="Q15" s="1">
         <v>34</v>
       </c>
     </row>
-    <row r="16" spans="2:17" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:17" x14ac:dyDescent="0.35">
       <c r="Q16" s="1">
         <v>4.26</v>
       </c>

</xml_diff>